<commit_message>
script completed for uploading data to db
</commit_message>
<xml_diff>
--- a/Sample Qs- Format for Script to Import Qs Ans.xlsx
+++ b/Sample Qs- Format for Script to Import Qs Ans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\Personal\IslamOnline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masaq\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7086668-7476-48CA-B896-86338544B3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE53368A-FF10-4245-8109-E90CD40B26C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B6473F29-DE04-4F01-9C1F-8F7758D6EB19}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{B6473F29-DE04-4F01-9C1F-8F7758D6EB19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample 3Qs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="102">
   <si>
     <t>تفسیر نعیمی ،ج3،ص252</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>حوالہ متن</t>
-  </si>
-  <si>
-    <t>سورہ آل عمران سے جواب</t>
   </si>
   <si>
     <t>B0031N003006</t>
@@ -105,9 +102,6 @@
     <t>B0031N003049</t>
   </si>
   <si>
-    <t xml:space="preserve">اختیارات انبیاء کرام </t>
-  </si>
-  <si>
     <t>Tauheed &amp; Shirk</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t xml:space="preserve"> اس آیت میں اللہ تعالیٰ نے اپنے حبیب   صَلَّی اللہُ تَعَالٰی عَلَیْہِ وَاٰلِہٖ وَسَلَّمَ  سے خطاب کرتے ہوئے ارشاد فرمایا کہ اے حبیب! صَلَّی اللہُ تَعَالٰی عَلَیْہِ وَاٰلِہٖ وَسَلَّمَ، حضرت نوح عَلَیْہِ الصَّلٰوۃُ وَالسَّلَام اور ان کی قوم کے جس واقعے کی ہم نے آپ کو خبر دی یہ غیب کی خبروں میں سے ہے جو ہم آپ کی طرف وحی کرتے ہیں۔ آپ پر قرآن نازل ہونے سے پہلے آپ اور آپ کی قوم ان غیبی خبروں کو تفصیل سے نہیں جانتی تھی لہٰذا اے حبیب! صَلَّی اللہُ تَعَالٰی عَلَیْہِ وَاٰلِہٖ وَسَلَّمَ ، جس طرح حضرت نوح   عَلَیْہِ الصَّلٰوۃُ وَالسَّلَام    نے اپنی قوم کی اذیتوں پر صبر کیا اسی طرح آپ بھی اپنی قوم کے مشرکین کی اذیتوں پر صبر کریں ، بے شک اچھا انجام یعنی دشمنوں کے خلاف مدد، فتح اور اُخروی سعادتوں کے حصول کے ذریعے کامیابی ایمان والوں کے لئے ہے۔</t>
   </si>
   <si>
-    <t>سورۃ ھود سے جواب</t>
-  </si>
-  <si>
     <t>کیا حضور ﷺ علمِ غیب جانتے تھے؟</t>
   </si>
   <si>
@@ -160,9 +151,6 @@
   </si>
   <si>
     <t>شان  نزول :ایک دن نبی اکرم ﷺنے فرمایا کہ  ’’میری امت کی پیدائش سے پہلے جب میری امت مٹی کی شکل میں تھی اس وقت وہ میرے سامنے اپنی صورتوں میں پیش کی گئی جیسا کہ حضرت آدم عَلَیْہِ الصَّلٰوۃُ وَالسَّلَام پر پیش کی گئی اور مجھے علم دیا گیا کہ کون مجھ پر ایمان لائے گا اور کون کفر کرے گا۔ یہ خبر جب منافقین کو پہنچی تو انہوں نے اِستِہزاء کے طور پر کہا کہ محمد مصطفٰی صَلَّی اللہُ تَعَالٰی عَلَیْہِ وَاٰلِہٖ وَسَلَّمَ کا گمان ہے کہ وہ یہ جانتے ہیں کہ جو لوگ ابھی پیدا بھی نہیں ہوئے ان میں سے کون ان پر ایمان لائے گا اورکون کفر کرے گا، جبکہ ہم ان کے ساتھ رہتے ہیں اور وہ ہمیں پہچانتے نہیں۔اس پر حضور سید المرسلین صَلَّی اللہُ تَعَالٰی عَلَیْہِ وَاٰلِہٖ وَسَلَّمَ منبر پر کھڑے ہوئے اور اللہ تعالیٰ کی حمد و ثنا کے بعد فرمایا ’’ان لوگوں کا کیا حال ہے جو میرے علم میں طعن (اعتراض) کرتے ہیں ، آج سے قیامت تک جو کچھ ہونے والا ہے اس میں سے کوئی چیز ایسی نہیں ہے جس کا تم مجھ سے سوال کرو اور میں تمہیں اس کی خبر نہ دے دوں۔ حضرت عبداللہ بن حذافہ سہمی رَضِیَ اللہُ تَعَالٰی عَنْہُ نے کھڑے ہو کر کہا: یا رسول اللہ!صَلَّی اللہُ تَعَالٰی عَلَیْہِ وَاٰلِہٖ وَسَلَّمَ ،میرا باپ کون ہے ؟ ارشاد فرمایا : حذافہ ،پھر حضرت عمر رَضِیَ اللہُ تَعَالٰی عَنْہُ نے کھڑے ہوکر عرض کی :یا رسول اللہ!صَلَّی اللہُ تَعَالٰی عَلَیْہِ وَاٰلِہٖ وَسَلَّمَ، ہم اللہ عَزَّوَجَلَّ کی ربوبیت پر راضی ہوئے، اسلام کے دین ہونے پر راضی ہوئے، قرآن کے امام و پیشواہونے پر راضی ہوئے ، آپ صَلَّی اللہُ تَعَالٰی عَلَیْہِ وَاٰلِہٖ وَسَلَّمَ کے نبی ہونے پر راضی ہوئے، ہم آپ صَلَّی اللہُ تَعَالٰی عَلَیْہِ وَاٰلِہٖ وَسَلَّمَ سے معافی چاہتے ہیں۔ تاجدارِ رسالت صَلَّی اللہُ تَعَالٰی عَلَیْہِ وَاٰلِہٖ وَسَلَّمَ  نے فرمایا: کیا تم باز آؤ گے؟ کیا تم باز آؤ گے؟ پھر منبر سے اتر آئے اس پراللہ  تعالیٰ نے یہ آیت نازل فرمائ</t>
-  </si>
-  <si>
-    <t>سورۃ آل عمران سے جواب</t>
   </si>
   <si>
     <t>اﷲ کی شان نہیں کہ اے عام لوگو! تمہیں غیب کا علم دے دے۔ ہاں اﷲ چن لیتا ہے اپنے رسولوں میں سے جسے چاہے۔</t>
@@ -185,9 +173,6 @@
 اس جیسی تمام آیات اور احادیث اس بات پر شاہد ہیں کہ آپ ﷺ کو علم غیب اللہ نے عطا فرمایا ہے اور اس کا اظہار بے شمار مواقع پر ہوا ۔</t>
   </si>
   <si>
-    <t>سورۃ بقرۃ سے جواب</t>
-  </si>
-  <si>
     <t>اور بات یوں ہی ہے کہ ہم نے تمہیں کیا سب امتوں میں افضل کہ تم لوگوں پر گواہ ہواور یہ رسول تمہارے نگہبان و گواہ</t>
   </si>
   <si>
@@ -215,9 +200,6 @@
   </si>
   <si>
     <t>علامہ سید نعیم الدین مراد آبادی رَحْمَۃُاللّٰہِ تَعَالٰی عَلَیْہِ  فرماتے ہیں :حضور نبی کریم ﷺرسولوں  میں  سب سے اعلیٰ ہیں ، اللّٰہ تعالیٰ نے آپ ﷺکو تمام اَشیاء کے علوم عطا فرمائے جیسا کہ صحاح کی معتبر اَحادیث سے ثابت ہے اور یہ آیت حضور (ﷺ) کے اور تمام مرتضیٰ رسولوں  کیلئے غیب کا علم ثابت کرتی ہے۔</t>
-  </si>
-  <si>
-    <t>سورۃ جن سے جواب</t>
   </si>
   <si>
     <t>Imaan &amp; Aqaaed</t>
@@ -304,9 +286,6 @@
     <t xml:space="preserve">ایاک نعبد وایاک نستعین </t>
   </si>
   <si>
-    <t>ایاک نعبد(سورۃ فاتحہ) سے استدلال</t>
-  </si>
-  <si>
     <t>B00013N001004</t>
   </si>
   <si>
@@ -320,9 +299,6 @@
   </si>
   <si>
     <t>فَكَیْفَ اِذَا جِئْنَا مِنْ كُلِّ اُمَّةٍۭ بِشَهِیْدٍ وَّ جِئْنَا بِكَ عَلٰى هٰۤؤُلَآءِ شَهِیْدًا</t>
-  </si>
-  <si>
-    <t>سورۃ النساء سے جواب</t>
   </si>
   <si>
     <t>B00012N004041</t>
@@ -392,9 +368,6 @@
     <t>یٰۤاَیُّهَا النَّبِیُّ اِنَّاۤ اَرْسَلْنٰكَ شَاهِدًا وَّ مُبَشِّرًا وَّ نَذِیْرًا</t>
   </si>
   <si>
-    <t>سورۃ احزاب سے جواب</t>
-  </si>
-  <si>
     <t>B00011N033073</t>
   </si>
   <si>
@@ -459,13 +432,34 @@
   </si>
   <si>
     <t>Q. No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> احزاب</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> النساء</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> جن</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> بقرۃ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> آل عمران</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ھود</t>
+  </si>
+  <si>
+    <t>فاتحہ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,6 +580,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -607,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -621,91 +621,85 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1044,697 +1038,921 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1"/>
   <cols>
-    <col min="7" max="7" width="50.109375" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="50.08984375" customWidth="1"/>
+    <col min="10" max="10" width="10.08984375" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="14" max="14" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="29" customFormat="1" ht="78">
-      <c r="A1" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="I1" s="29" t="s">
+    <row r="1" spans="1:16" s="20" customFormat="1" ht="62">
+      <c r="A1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="26" customHeight="1">
+      <c r="A2" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A3" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="M1" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="N1" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="O1" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="P1" s="29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="27.6">
-      <c r="A2" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="27.6" outlineLevel="1">
-      <c r="A3" s="27"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>79</v>
+      <c r="G3" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="N3" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="27.6" outlineLevel="1">
-      <c r="A4" s="27"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="5"/>
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A4" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="143" outlineLevel="1">
+      <c r="A5" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="151.80000000000001" outlineLevel="1">
-      <c r="A5" s="27"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="F5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A6" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" ht="27.6" outlineLevel="1">
-      <c r="A6" s="27"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="5"/>
       <c r="F6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>72</v>
+      <c r="G6" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="N6" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="27.6" outlineLevel="1">
-      <c r="A7" s="27"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="5"/>
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A7" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="F7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="151.80000000000001" outlineLevel="1">
-      <c r="A8" s="27"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="N7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="130" outlineLevel="1">
+      <c r="A8" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="F8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="15" t="s">
         <v>63</v>
       </c>
+      <c r="H8" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="M8" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" ht="27.6" outlineLevel="1">
-      <c r="A9" s="27"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="N8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A9" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="F9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>66</v>
+      <c r="G9" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="N9" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="27.6" outlineLevel="1">
-      <c r="A10" s="27"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="5"/>
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A10" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>3</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" ht="179.4" outlineLevel="1">
-      <c r="A11" s="27"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="1" customFormat="1" ht="169" outlineLevel="1">
+      <c r="A11" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="F11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>63</v>
+      <c r="G11" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="M11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="65">
+      <c r="A12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" ht="82.8">
-      <c r="A12" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>19</v>
+        <v>53</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="M12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="36.6" outlineLevel="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="5"/>
       <c r="F13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="N13" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" ht="36.6" outlineLevel="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="5"/>
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="15"/>
+        <v>49</v>
+      </c>
+      <c r="H14" s="9"/>
       <c r="M14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N14" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="52" outlineLevel="1">
+      <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="55.2" outlineLevel="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="5"/>
       <c r="F15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" ht="36.6" outlineLevel="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="N15" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" s="1" customFormat="1" ht="36.6" outlineLevel="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="5"/>
+      <c r="D17" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F17" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" s="1" customFormat="1" ht="151.80000000000001" outlineLevel="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="5"/>
+      <c r="N17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="1" customFormat="1" ht="130" outlineLevel="1">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F18" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" s="1" customFormat="1" ht="36.6" outlineLevel="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="N18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" s="1" customFormat="1" ht="36.6" outlineLevel="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F20" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" s="16" customFormat="1" ht="138" outlineLevel="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="19" t="s">
+      <c r="N20" s="1">
         <v>2</v>
       </c>
-      <c r="G21" s="18" t="s">
+    </row>
+    <row r="21" spans="1:14" s="10" customFormat="1" ht="130" outlineLevel="1">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="1" customFormat="1" ht="36.6" outlineLevel="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="D21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="N21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="D22" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="1" customFormat="1" ht="36.6" outlineLevel="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="D23" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F23" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" s="1" customFormat="1" ht="289.8" outlineLevel="1">
-      <c r="A24" s="8"/>
-      <c r="B24" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="12" t="s">
+      <c r="N23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="1" customFormat="1" ht="273" outlineLevel="1">
+      <c r="A24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="D24" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F24" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="1" customFormat="1" ht="36.6" outlineLevel="1">
-      <c r="A25" s="8"/>
-      <c r="B25" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" s="1" customFormat="1" ht="36.6" outlineLevel="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="12" t="s">
+      <c r="H25" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="N25" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="1" customFormat="1" ht="36" outlineLevel="1">
+      <c r="A26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F26" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N26" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="1" customFormat="1" ht="130" outlineLevel="1">
+      <c r="A27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" s="1" customFormat="1" ht="138" outlineLevel="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="5"/>
+      <c r="D27" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F27" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" s="1" customFormat="1" ht="69" outlineLevel="1">
-      <c r="A28" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="H27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="N27" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="1" customFormat="1" ht="65" outlineLevel="1">
+      <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="B28" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N28" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="1" customFormat="1" ht="13" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="3" t="s">
+      <c r="C29" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H28" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" s="1" customFormat="1" ht="27.6">
-      <c r="A29" s="8"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="5"/>
       <c r="F29" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N29" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="1" customFormat="1" ht="36">
+      <c r="A30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H29" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" s="1" customFormat="1" ht="27.6">
-      <c r="A30" s="8"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="5"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F30" s="4" t="s">
         <v>5</v>
       </c>
@@ -1742,68 +1960,110 @@
         <f>G2</f>
         <v xml:space="preserve">جی ہاں نبی اکرم ﷺ حاضر بھی ہیں اور ناظر بھی اس کا جواز آیت قرآنی اور احادیث سے ثابت ہے </v>
       </c>
-      <c r="H30" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" s="1" customFormat="1" ht="331.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="5"/>
+      <c r="H30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="1" customFormat="1" ht="312">
+      <c r="A31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="30"/>
+      <c r="E31" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F31" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" s="1" customFormat="1" ht="13.8">
-      <c r="A32" s="8"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="6" t="s">
+      <c r="H31" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="N31" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="1" customFormat="1" ht="36">
+      <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="D32" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F32" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" s="1" customFormat="1" ht="27.6">
-      <c r="A33" s="8"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="5"/>
+      <c r="N32" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" s="1" customFormat="1" ht="36">
+      <c r="A33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="31"/>
+      <c r="E33" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F33" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="H33" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" s="1" customFormat="1" ht="179.4">
-      <c r="A34" s="8"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="5"/>
+      <c r="N33" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="1" customFormat="1" ht="169">
+      <c r="A34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="31"/>
+      <c r="E34" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F34" s="4" t="s">
         <v>2</v>
       </c>
@@ -1813,33 +2073,18 @@
       <c r="H34" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="N34" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="E2:E11"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="C6:C8"/>
+  <mergeCells count="4">
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D32:D34"/>
     <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
-    <mergeCell ref="A12:A27"/>
-    <mergeCell ref="E12:E27"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="E28:E34"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="D32:D34"/>
   </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>